<commit_message>
un petit changement dans la matrice
</commit_message>
<xml_diff>
--- a/Remise/Documentation_technique/matrice_verification.xlsx
+++ b/Remise/Documentation_technique/matrice_verification.xlsx
@@ -174,7 +174,7 @@
     <t>t=0.2s pour une charge du banc de condensateur d'environs 1500V</t>
   </si>
   <si>
-    <t>t=0.2s, Pmoy = 2.52MW et Pmax=3.8MW pour PSIM, Pmoy=%%MW et Pmax=%%MW pour SPS</t>
+    <t>t=0.2s, Pmoy = 2.53MW et Pmax=3.8MW pour PSIM, Pmoy=2.62MW et Pmax=4.3MW pour SPS</t>
   </si>
 </sst>
 </file>
@@ -350,18 +350,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -375,6 +363,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,8 +400,8 @@
       <xdr:rowOff>71437</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1"/>
@@ -437,6 +437,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -472,7 +473,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1"/>
@@ -538,8 +539,8 @@
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="ZoneTexte 2"/>
@@ -575,6 +576,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -610,7 +612,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="ZoneTexte 2"/>
@@ -676,8 +678,8 @@
       <xdr:rowOff>238125</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="ZoneTexte 3"/>
@@ -713,6 +715,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -748,7 +751,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="ZoneTexte 3"/>
@@ -814,8 +817,8 @@
       <xdr:rowOff>285750</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="ZoneTexte 4"/>
@@ -851,6 +854,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -886,7 +890,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="ZoneTexte 4"/>
@@ -947,7 +951,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
@@ -961,7 +965,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8334375" y="2095500"/>
+              <a:off x="8420100" y="2095500"/>
               <a:ext cx="914400" cy="264560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -989,6 +993,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1032,7 +1037,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8334375" y="2095500"/>
+              <a:off x="8420100" y="2095500"/>
               <a:ext cx="914400" cy="264560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1060,6 +1065,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="fr-CA" sz="1100" i="0">
                   <a:latin typeface="Cambria Math"/>
@@ -1090,8 +1096,8 @@
       <xdr:rowOff>381000</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="ZoneTexte 6"/>
@@ -1127,6 +1133,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1162,7 +1169,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="ZoneTexte 6"/>
@@ -1223,9 +1230,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>190499</xdr:colOff>
+      <xdr:colOff>133349</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>242887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1362076" cy="264560"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1237,7 +1244,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8362949" y="4043362"/>
+              <a:off x="8305799" y="4195762"/>
               <a:ext cx="1362076" cy="264560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1297,7 +1304,7 @@
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -1309,7 +1316,7 @@
                         <a:schemeClr val="tx1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -1333,7 +1340,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8362949" y="4043362"/>
+              <a:off x="8305799" y="4195762"/>
               <a:ext cx="1362076" cy="264560"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1391,7 +1398,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1403,7 +1410,7 @@
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:effectLst/>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Cambria Math"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
@@ -1428,8 +1435,8 @@
       <xdr:rowOff>485775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1362076" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="ZoneTexte 8"/>
@@ -1465,6 +1472,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1516,7 +1524,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="ZoneTexte 8"/>
@@ -1605,8 +1613,8 @@
       <xdr:rowOff>214312</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="581025" cy="609013"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="ZoneTexte 9"/>
@@ -1690,7 +1698,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="ZoneTexte 9"/>
@@ -2066,7 +2074,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,7 +2115,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="3.5">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2119,11 +2127,11 @@
       <c r="D2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="9" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="4" t="s">
@@ -2131,7 +2139,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2141,7 +2149,7 @@
       <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4" t="s">
         <v>46</v>
       </c>
@@ -2151,7 +2159,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2163,15 +2171,15 @@
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
@@ -2181,15 +2189,15 @@
       <c r="D5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2199,15 +2207,15 @@
       <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2219,7 +2227,7 @@
       <c r="D7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="7" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -2231,7 +2239,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
@@ -2241,7 +2249,7 @@
       <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="4"/>
@@ -2249,7 +2257,7 @@
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2261,7 +2269,7 @@
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="4" t="s">
         <v>47</v>
       </c>
@@ -2269,7 +2277,7 @@
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
@@ -2279,7 +2287,7 @@
       <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="11"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="4" t="s">
         <v>47</v>
       </c>
@@ -2287,7 +2295,7 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2299,7 +2307,7 @@
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="7"/>
       <c r="F11" s="4" t="s">
         <v>48</v>
       </c>
@@ -2307,7 +2315,7 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
@@ -2317,7 +2325,7 @@
       <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="4" t="s">
         <v>48</v>
       </c>
@@ -2325,7 +2333,7 @@
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:8" ht="63" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
@@ -2335,7 +2343,7 @@
       <c r="D13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="4" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Changement de la commande
Mise de la nouvelle commande pour AFE 3 niveaux. AFE+DCP/DCN de PSIM et
AFE+DCP/DCN de SPS.
Changement de la limite de courant à 800 pour ses simulations à cause de
la plus grande efficacité de la commande pour respecter la limite de
puissance maximal.
</commit_message>
<xml_diff>
--- a/Remise/Documentation_technique/matrice_verification.xlsx
+++ b/Remise/Documentation_technique/matrice_verification.xlsx
@@ -171,10 +171,10 @@
     <t>Des changement ne compromettant pas la stabilité du système ont été testé</t>
   </si>
   <si>
-    <t>t=0.2s pour une charge du banc de condensateur d'environs 1500V</t>
-  </si>
-  <si>
-    <t>t=0.2s, Pmoy = 2.53MW et Pmax=3.8MW pour PSIM, Pmoy=2.62MW et Pmax=4.3MW pour SPS</t>
+    <t>t=0.31s pour une charge du banc de condensateur d'environs 1700V</t>
+  </si>
+  <si>
+    <t>t=0.31s, Pmoy = 2.53MW et Pmax=3.55MW pour PSIM, Pmoy=2.58MW et Pmax=3.56MW pour SPS</t>
   </si>
 </sst>
 </file>
@@ -956,8 +956,8 @@
       <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="ZoneTexte 5"/>
@@ -1029,7 +1029,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="ZoneTexte 5"/>
@@ -1235,8 +1235,8 @@
       <xdr:rowOff>242887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1362076" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="ZoneTexte 7"/>
@@ -1332,7 +1332,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="ZoneTexte 7"/>
@@ -2073,7 +2073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>

</xml_diff>